<commit_message>
Update weather reporting to use arrays; add score evaluation
</commit_message>
<xml_diff>
--- a/Crop Summary.xlsx
+++ b/Crop Summary.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Crop</t>
   </si>
@@ -36,9 +36,6 @@
     <t>Ideal heat</t>
   </si>
   <si>
-    <t>Yield factor</t>
-  </si>
-  <si>
     <t>Mean</t>
   </si>
   <si>
@@ -52,6 +49,21 @@
   </si>
   <si>
     <t>Summary</t>
+  </si>
+  <si>
+    <t>Wet Fac</t>
+  </si>
+  <si>
+    <t>Heat Fac</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>Scaling</t>
+  </si>
+  <si>
+    <t>Potato</t>
   </si>
 </sst>
 </file>
@@ -124,13 +136,7 @@
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="4" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="4" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -139,6 +145,12 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="4" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -453,63 +465,91 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5C7D548-A478-46BE-A258-72079E23A6AA}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8" customWidth="1"/>
-    <col min="2" max="2" width="9.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.28515625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="5"/>
-    <col min="7" max="7" width="12.7109375" style="8" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="9.85546875" style="5" customWidth="1"/>
+    <col min="7" max="7" width="11" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.28515625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="3"/>
+    <col min="10" max="10" width="12.7109375" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="3" t="s">
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>8</v>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="5">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C3" s="5">
+        <v>0.9</v>
+      </c>
+      <c r="J3" s="6" t="str">
+        <f>H3&amp;" +/- "&amp;I3</f>
+        <v xml:space="preserve"> +/- </v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="H1:J1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Revise yield calculation, add new crops, balance difficulty/yields
</commit_message>
<xml_diff>
--- a/Crop Summary.xlsx
+++ b/Crop Summary.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Dropbox\Projects\Programming\Java\Eclipse\ACS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Projects\Programming\Java\Eclipse\ACS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{AD194676-4100-4EBB-8894-89FD8AEAE776}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{BE919D53-09FD-46FE-B214-FF41D901BD52}"/>
   </bookViews>
   <sheets>
-    <sheet name="Parameters" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="171027"/>
-  <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,45 +24,117 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Crop</t>
   </si>
   <si>
-    <t>Ideal wet</t>
-  </si>
-  <si>
-    <t>Ideal heat</t>
+    <t>Description Text</t>
+  </si>
+  <si>
+    <t>IW</t>
+  </si>
+  <si>
+    <t>WF</t>
+  </si>
+  <si>
+    <t>IH</t>
+  </si>
+  <si>
+    <t>HF</t>
+  </si>
+  <si>
+    <t>Cost</t>
+  </si>
+  <si>
+    <t>Sale</t>
+  </si>
+  <si>
+    <t>Exp. Perf.</t>
+  </si>
+  <si>
+    <t>Meta</t>
+  </si>
+  <si>
+    <t>Factors</t>
+  </si>
+  <si>
+    <t>Potato</t>
+  </si>
+  <si>
+    <t>Starchy tuber of the nightshade family prized for caloric content. Thrives in cool, wet weather.</t>
+  </si>
+  <si>
+    <t>Carrot</t>
+  </si>
+  <si>
+    <t>Parsnip</t>
+  </si>
+  <si>
+    <t>Turnip</t>
+  </si>
+  <si>
+    <t>Wheat</t>
+  </si>
+  <si>
+    <t>Corn</t>
+  </si>
+  <si>
+    <t>Tomato</t>
+  </si>
+  <si>
+    <t>Blueberry</t>
+  </si>
+  <si>
+    <t>Pumpkin</t>
   </si>
   <si>
     <t>Mean</t>
   </si>
   <si>
-    <t>Stdev</t>
-  </si>
-  <si>
-    <t>Inputs</t>
-  </si>
-  <si>
-    <t>Performance</t>
-  </si>
-  <si>
-    <t>Summary</t>
-  </si>
-  <si>
-    <t>Wet Fac</t>
-  </si>
-  <si>
-    <t>Heat Fac</t>
-  </si>
-  <si>
-    <t>Max</t>
-  </si>
-  <si>
-    <t>Scaling</t>
-  </si>
-  <si>
-    <t>Potato</t>
+    <t>SD</t>
+  </si>
+  <si>
+    <t>SD Bounds</t>
+  </si>
+  <si>
+    <t>+1</t>
+  </si>
+  <si>
+    <t>Nutritious root vegetable which prefers plenty of sunlight.</t>
+  </si>
+  <si>
+    <t>Tasty root vegetable which is spoiled by excessive rain.</t>
+  </si>
+  <si>
+    <t>Reliable root vegetable which loves temperate climates.</t>
+  </si>
+  <si>
+    <t>Grass cultivated worldwide for its starchy cereal grains. Grows well in most weather.</t>
+  </si>
+  <si>
+    <t>Profitable grain plant requiring warm and wet weather.</t>
+  </si>
+  <si>
+    <t>Juicy fruit of the nightshade family requiring warmth and plenty of sun.</t>
+  </si>
+  <si>
+    <t>Grape</t>
+  </si>
+  <si>
+    <t>An expensive and tricky berry growing best in warm, dry climates. Potentially very valuable.</t>
+  </si>
+  <si>
+    <t>Delicious and popular berry damaged by heavy rain.</t>
+  </si>
+  <si>
+    <t>Squash plant prized for decoration. Prefers warm weather and some rain.</t>
+  </si>
+  <si>
+    <t>Avg profit / 100</t>
+  </si>
+  <si>
+    <t>Cost / 100</t>
   </si>
 </sst>
 </file>
@@ -71,9 +142,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="#,##0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -89,8 +160,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -105,19 +184,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="-0.499984740745262"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -134,21 +201,31 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="4" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="4" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -464,93 +541,644 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5C7D548-A478-46BE-A258-72079E23A6AA}">
-  <dimension ref="A1:J3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D22EF5B-26CD-46A6-9D20-461BE1875E7E}">
+  <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8" customWidth="1"/>
-    <col min="2" max="2" width="9.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="9.85546875" style="5" customWidth="1"/>
-    <col min="7" max="7" width="11" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.28515625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="3"/>
-    <col min="10" max="10" width="12.7109375" style="6" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="86.5703125" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="8"/>
+    <col min="9" max="10" width="9.140625" style="4"/>
+    <col min="11" max="11" width="15.140625" style="2" customWidth="1"/>
+    <col min="12" max="13" width="9.140625" style="4"/>
+    <col min="14" max="14" width="9.140625" style="8"/>
+    <col min="15" max="15" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
+    <row r="1" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="M1" s="13"/>
+      <c r="N1" s="9"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" s="12"/>
+      <c r="L2" s="5">
+        <v>-1</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="N2" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3">
+        <v>1.05</v>
+      </c>
+      <c r="D3">
+        <v>0.5</v>
+      </c>
+      <c r="E3">
+        <v>1.05</v>
+      </c>
+      <c r="F3">
+        <v>0.5</v>
+      </c>
+      <c r="G3">
+        <v>5</v>
+      </c>
+      <c r="H3" s="8">
+        <v>7</v>
+      </c>
+      <c r="I3" s="4">
+        <v>0.91</v>
+      </c>
+      <c r="J3" s="4">
+        <v>4.7E-2</v>
+      </c>
+      <c r="K3" s="2" t="str">
+        <f>ROUND((H3/G3*I3),2)&amp;" +/- "&amp;ROUND((H3/G3*J3), 3)</f>
+        <v>1.27 +/- 0.066</v>
+      </c>
+      <c r="L3" s="4">
+        <f>(I3-J3)*(H3/G3)</f>
+        <v>1.2081999999999999</v>
+      </c>
+      <c r="M3" s="4">
+        <f>(I3+J3)*(H3/G3)</f>
+        <v>1.3398000000000001</v>
+      </c>
+      <c r="N3" s="8">
+        <f>G3*100</f>
+        <v>500</v>
+      </c>
+      <c r="O3">
+        <f>100*(H3-G3)*I3</f>
+        <v>182</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>0.8</v>
+      </c>
+      <c r="E4">
+        <v>0.9</v>
+      </c>
+      <c r="F4">
+        <v>0.8</v>
+      </c>
+      <c r="G4">
+        <v>6</v>
+      </c>
+      <c r="H4" s="8">
+        <v>9</v>
+      </c>
+      <c r="I4" s="4">
+        <v>0.86</v>
+      </c>
+      <c r="J4" s="4">
+        <v>7.0400000000000004E-2</v>
+      </c>
+      <c r="K4" s="2" t="str">
+        <f>ROUND((H4/G4*I4),2)&amp;" +/- "&amp;ROUND((H4/G4*J4), 3)</f>
+        <v>1.29 +/- 0.106</v>
+      </c>
+      <c r="L4" s="4">
+        <f>(I4-J4)*(H4/G4)</f>
+        <v>1.1843999999999999</v>
+      </c>
+      <c r="M4" s="4">
+        <f>(I4+J4)*(H4/G4)</f>
+        <v>1.3956</v>
+      </c>
+      <c r="N4" s="8">
+        <f t="shared" ref="N4:N12" si="0">G4*100</f>
+        <v>600</v>
+      </c>
+      <c r="O4">
+        <f>100*(H4-G4)*I4</f>
+        <v>258</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D5">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E5">
+        <v>0.9</v>
+      </c>
+      <c r="F5">
+        <v>0.7</v>
+      </c>
+      <c r="G5">
         <v>8</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="H5" s="8">
+        <v>14</v>
+      </c>
+      <c r="I5" s="4">
+        <v>0.79</v>
+      </c>
+      <c r="J5" s="4">
+        <v>0.10440000000000001</v>
+      </c>
+      <c r="K5" s="2" t="str">
+        <f>ROUND((H5/G5*I5),2)&amp;" +/- "&amp;ROUND((H5/G5*J5), 3)</f>
+        <v>1.38 +/- 0.183</v>
+      </c>
+      <c r="L5" s="4">
+        <f>(I5-J5)*(H5/G5)</f>
+        <v>1.1998</v>
+      </c>
+      <c r="M5" s="4">
+        <f>(I5+J5)*(H5/G5)</f>
+        <v>1.5652000000000001</v>
+      </c>
+      <c r="N5" s="8">
+        <f t="shared" si="0"/>
+        <v>800</v>
+      </c>
+      <c r="O5">
+        <f>100*(H5-G5)*I5</f>
+        <v>474</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>0.8</v>
+      </c>
+      <c r="E6">
+        <v>1.2</v>
+      </c>
+      <c r="F6">
+        <v>1.2</v>
+      </c>
+      <c r="G6">
         <v>9</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="4" t="s">
+      <c r="H6" s="8">
+        <v>18</v>
+      </c>
+      <c r="I6" s="4">
+        <v>0.69</v>
+      </c>
+      <c r="J6" s="4">
+        <v>0.1263</v>
+      </c>
+      <c r="K6" s="2" t="str">
+        <f t="shared" ref="K6:K7" si="1">ROUND((H6/G6*I6),2)&amp;" +/- "&amp;ROUND((H6/G6*J6), 3)</f>
+        <v>1.38 +/- 0.253</v>
+      </c>
+      <c r="L6" s="4">
+        <f>(I6-J6)*(H6/G6)</f>
+        <v>1.1274</v>
+      </c>
+      <c r="M6" s="4">
+        <f>(I6+J6)*(H6/G6)</f>
+        <v>1.6325999999999998</v>
+      </c>
+      <c r="N6" s="8">
+        <f t="shared" si="0"/>
+        <v>900</v>
+      </c>
+      <c r="O6">
+        <f t="shared" ref="O6:O12" si="2">100*(H6-G6)*I6</f>
+        <v>621</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7">
+        <v>0.9</v>
+      </c>
+      <c r="D7">
+        <v>1.2</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>0.8</v>
+      </c>
+      <c r="G7">
+        <v>9</v>
+      </c>
+      <c r="H7" s="8">
+        <v>17</v>
+      </c>
+      <c r="I7" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="J7" s="4">
+        <v>0.12379999999999999</v>
+      </c>
+      <c r="K7" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>1.32 +/- 0.234</v>
+      </c>
+      <c r="L7" s="4">
+        <f t="shared" ref="L7" si="3">(I7-J7)*(H7/G7)</f>
+        <v>1.0883777777777777</v>
+      </c>
+      <c r="M7" s="4">
+        <f t="shared" ref="M7" si="4">(I7+J7)*(H7/G7)</f>
+        <v>1.5560666666666665</v>
+      </c>
+      <c r="N7" s="8">
+        <f t="shared" si="0"/>
+        <v>900</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="2"/>
+        <v>560</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>0.5</v>
+      </c>
+      <c r="E8">
+        <v>1.2</v>
+      </c>
+      <c r="F8">
+        <v>1.3</v>
+      </c>
+      <c r="G8">
+        <v>9</v>
+      </c>
+      <c r="H8" s="8">
+        <v>17</v>
+      </c>
+      <c r="I8" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="J8" s="4">
+        <v>0.12970000000000001</v>
+      </c>
+      <c r="K8" s="2" t="str">
+        <f>ROUND((H8/G8*I8),2)&amp;" +/- "&amp;ROUND((H8/G8*J8), 3)</f>
+        <v>1.32 +/- 0.245</v>
+      </c>
+      <c r="L8" s="4">
+        <f>(I8-J8)*(H8/G8)</f>
+        <v>1.077233333333333</v>
+      </c>
+      <c r="M8" s="4">
+        <f>(I8+J8)*(H8/G8)</f>
+        <v>1.5672111111111111</v>
+      </c>
+      <c r="N8" s="8">
+        <f t="shared" si="0"/>
+        <v>900</v>
+      </c>
+      <c r="O8">
+        <f>100*(H8-G8)*I8</f>
+        <v>560</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="F9">
+        <v>1.3</v>
+      </c>
+      <c r="G9">
         <v>11</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>7</v>
+      <c r="H9" s="8">
+        <v>26</v>
+      </c>
+      <c r="I9" s="4">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="J9" s="4">
+        <v>0.1285</v>
+      </c>
+      <c r="K9" s="2" t="str">
+        <f t="shared" ref="K9:K12" si="5">ROUND((H9/G9*I9),2)&amp;" +/- "&amp;ROUND((H9/G9*J9), 3)</f>
+        <v>1.37 +/- 0.304</v>
+      </c>
+      <c r="L9" s="4">
+        <f t="shared" ref="L9:L12" si="6">(I9-J9)*(H9/G9)</f>
+        <v>1.0671818181818182</v>
+      </c>
+      <c r="M9" s="4">
+        <f t="shared" ref="M9:M12" si="7">(I9+J9)*(H9/G9)</f>
+        <v>1.6746363636363635</v>
+      </c>
+      <c r="N9" s="8">
+        <f t="shared" si="0"/>
+        <v>1100</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="2"/>
+        <v>869.99999999999989</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="5">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10">
+        <v>0.8</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>0.7</v>
+      </c>
+      <c r="G10">
+        <v>13</v>
+      </c>
+      <c r="H10" s="8">
+        <v>30</v>
+      </c>
+      <c r="I10" s="4">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="J10" s="4">
+        <v>0.1963</v>
+      </c>
+      <c r="K10" s="2" t="str">
+        <f>ROUND((H10/G10*I10),2)&amp;" +/- "&amp;ROUND((H10/G10*J10), 3)</f>
+        <v>1.27 +/- 0.453</v>
+      </c>
+      <c r="L10" s="4">
+        <f>(I10-J10)*(H10/G10)</f>
+        <v>0.8162307692307692</v>
+      </c>
+      <c r="M10" s="4">
+        <f>(I10+J10)*(H10/G10)</f>
+        <v>1.7222307692307692</v>
+      </c>
+      <c r="N10" s="8">
+        <f t="shared" si="0"/>
+        <v>1300</v>
+      </c>
+      <c r="O10">
+        <f>100*(H10-G10)*I10</f>
+        <v>935.00000000000011</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11">
+        <v>0.8</v>
+      </c>
+      <c r="D11">
         <v>1.1000000000000001</v>
       </c>
-      <c r="C3" s="5">
-        <v>0.9</v>
-      </c>
-      <c r="J3" s="6" t="str">
-        <f>H3&amp;" +/- "&amp;I3</f>
-        <v xml:space="preserve"> +/- </v>
+      <c r="E11">
+        <v>1.2</v>
+      </c>
+      <c r="F11">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G11">
+        <v>18</v>
+      </c>
+      <c r="H11" s="8">
+        <v>45</v>
+      </c>
+      <c r="I11" s="4">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="J11" s="4">
+        <v>0.15040000000000001</v>
+      </c>
+      <c r="K11" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>1.38 +/- 0.376</v>
+      </c>
+      <c r="L11" s="4">
+        <f t="shared" si="6"/>
+        <v>0.99900000000000011</v>
+      </c>
+      <c r="M11" s="4">
+        <f t="shared" si="7"/>
+        <v>1.7510000000000001</v>
+      </c>
+      <c r="N11" s="8">
+        <f t="shared" si="0"/>
+        <v>1800</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="2"/>
+        <v>1485.0000000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>21</v>
+      </c>
+      <c r="H12" s="8">
+        <v>37</v>
+      </c>
+      <c r="I12" s="4">
+        <v>0.77</v>
+      </c>
+      <c r="J12" s="4">
+        <v>0.1132</v>
+      </c>
+      <c r="K12" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>1.36 +/- 0.199</v>
+      </c>
+      <c r="L12" s="4">
+        <f t="shared" si="6"/>
+        <v>1.1572190476190476</v>
+      </c>
+      <c r="M12" s="4">
+        <f t="shared" si="7"/>
+        <v>1.5561142857142856</v>
+      </c>
+      <c r="N12" s="8">
+        <f t="shared" si="0"/>
+        <v>2100</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="2"/>
+        <v>1232</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="H1:J1"/>
+  <mergeCells count="4">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="C1:J1"/>
+    <mergeCell ref="L1:M1"/>
   </mergeCells>
+  <conditionalFormatting sqref="C1:C1048576">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E1:E1048576">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF5A8AC6"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>